<commit_message>
Changes on xlsx test
</commit_message>
<xml_diff>
--- a/UX-test/approve-reject/flow-assets-test.xlsx
+++ b/UX-test/approve-reject/flow-assets-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anagrana/Documents/Kactus/design-system/UX-test/approve-reject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylmejia/Documents/Repo/design-system/design-system/UX-test/approve-reject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{038C7B7D-3FAF-6E45-886E-395F23D25F7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F1591C-151D-4844-B3EB-53A23E0AF1D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14500" yWindow="7340" windowWidth="28320" windowHeight="17840" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="28440" windowHeight="18720" xr2:uid="{69B89F32-9673-BB49-9CD2-9562BEC1F27F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Tasks</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Flow interacting with assets on Assets-explorer page</t>
   </si>
   <si>
-    <t>Go to the "Upload assets" button and upload luigi.jpg image.</t>
-  </si>
-  <si>
     <t>Tell us how many assets are and describe for each one how many aproves, rejects and comments are</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aprove o reject the asset that has been uploaded </t>
+  </si>
+  <si>
+    <t>Upload the donkey.jpg image of xxxxx folder in the project nintendo.</t>
   </si>
   <si>
     <r>
@@ -66,7 +66,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>mushroom.jpg</t>
+      <t>Bowser.jpg</t>
     </r>
     <r>
       <rPr>
@@ -89,7 +89,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">peach.jpg
+      <t xml:space="preserve">Yoshi.jpg
 </t>
     </r>
     <r>
@@ -102,9 +102,6 @@
       </rPr>
       <t>Aproved:        Rejected:          Comments:</t>
     </r>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -277,6 +274,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,21 +297,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -319,7 +316,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -615,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657FE3D-C789-FA47-A22F-70453D6154E9}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,14 +624,14 @@
     <col min="3" max="3" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -645,64 +642,59 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+    <row r="3" spans="1:3" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>8</v>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>8</v>
+    <row r="6" spans="1:3" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="151" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="7" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F14" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>